<commit_message>
Small typo fix that was preventing the CmpStdStk table from rendering in the Describe Tables menu.
git-svn-id: svn+ssh://svn.code.sf.net/p/open-fvs/code/rFVS@3220 90b89b48-9230-0de4-5065-812dd12741b8
</commit_message>
<xml_diff>
--- a/shinyFVSDataConvert/databaseDescription.xlsx
+++ b/shinyFVSDataConvert/databaseDescription.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Open-FVS\rFVS\shinyFVSOnlineDev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\FVS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB14DBD-B35F-41D6-8A99-955FE94C813D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C062CD-FE47-4BFA-A71D-37D0CC8E0365}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="47" activeTab="50" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OutputTableDescriptions" sheetId="1" r:id="rId1"/>
@@ -65,8 +65,8 @@
     <sheet name="FVS_TreeInit" sheetId="48" r:id="rId50"/>
     <sheet name="CmpMetaData" sheetId="49" r:id="rId51"/>
     <sheet name="CmpCompute" sheetId="54" r:id="rId52"/>
-    <sheet name="CmpStdStck" sheetId="55" r:id="rId53"/>
-    <sheet name="CmpStdStck_East" sheetId="56" r:id="rId54"/>
+    <sheet name="CmpStdStk" sheetId="55" r:id="rId53"/>
+    <sheet name="CmpStdStk_East" sheetId="56" r:id="rId54"/>
     <sheet name="CmpSummary" sheetId="50" r:id="rId55"/>
     <sheet name="CmpSummary_East" sheetId="51" r:id="rId56"/>
     <sheet name="CmpSummary2" sheetId="52" r:id="rId57"/>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4853" uniqueCount="1918">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4863" uniqueCount="1918">
   <si>
     <t>Table</t>
   </si>
@@ -10136,8 +10136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E862E947-F1E6-43BF-9C6E-9E8C99A65D26}">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10246,13 +10246,17 @@
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="20"/>
+      <c r="B13" s="20" t="s">
+        <v>1907</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="20"/>
+      <c r="B14" s="20" t="s">
+        <v>1907</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
@@ -10482,48 +10486,72 @@
       <c r="A43" s="1" t="s">
         <v>84</v>
       </c>
+      <c r="B43" s="20" t="s">
+        <v>1907</v>
+      </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B44" t="s">
-        <v>27</v>
+      <c r="B44" s="20" t="s">
+        <v>1907</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>88</v>
       </c>
+      <c r="B45" s="20" t="s">
+        <v>1907</v>
+      </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>90</v>
       </c>
+      <c r="B46" s="20" t="s">
+        <v>1907</v>
+      </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>92</v>
       </c>
+      <c r="B47" s="20" t="s">
+        <v>1907</v>
+      </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B48" s="20" t="s">
+        <v>1907</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B49" s="20" t="s">
+        <v>1907</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>1862</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B50" s="20" t="s">
+        <v>1907</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>1903</v>
+      </c>
+      <c r="B51" s="20" t="s">
+        <v>1907</v>
       </c>
     </row>
   </sheetData>
@@ -10567,9 +10595,20 @@
     <hyperlink ref="B41" r:id="rId37" xr:uid="{4E5BE34D-B570-4432-8F4B-92CFCEA1F3D1}"/>
     <hyperlink ref="B42" r:id="rId38" xr:uid="{F69B7270-052E-4DFD-890E-A9FDAD0A0165}"/>
     <hyperlink ref="B29" r:id="rId39" xr:uid="{3A4A1B09-5715-4CDC-A70D-7E4E5995FF73}"/>
+    <hyperlink ref="B13" r:id="rId40" xr:uid="{1F4A1F46-B3DB-4E50-8C9C-0CCCB1D924D3}"/>
+    <hyperlink ref="B14" r:id="rId41" xr:uid="{7169CC68-0E8C-4E85-8017-12EC143C5EEC}"/>
+    <hyperlink ref="B43" r:id="rId42" xr:uid="{9946F1C6-696C-4E8A-8435-291E3BEBAEA4}"/>
+    <hyperlink ref="B44" r:id="rId43" xr:uid="{6CA0E969-5243-4037-93A0-6EDB9F10DC6D}"/>
+    <hyperlink ref="B45" r:id="rId44" xr:uid="{54746D16-6912-41B6-8E5C-9142C0901FAE}"/>
+    <hyperlink ref="B46" r:id="rId45" xr:uid="{FBEEAC59-734E-420E-B5FF-ADEADAEC0523}"/>
+    <hyperlink ref="B47" r:id="rId46" xr:uid="{906073E0-3B8C-4C90-98BA-51F3BEDD8534}"/>
+    <hyperlink ref="B48" r:id="rId47" xr:uid="{BA6DFF66-0EED-43A5-AD66-10F07DBA6B3B}"/>
+    <hyperlink ref="B49" r:id="rId48" xr:uid="{5525272D-07FD-4C30-9B17-F06BF94C185F}"/>
+    <hyperlink ref="B50" r:id="rId49" xr:uid="{C8D4FF92-F9AB-4240-A616-31761110F851}"/>
+    <hyperlink ref="B51" r:id="rId50" xr:uid="{906A66ED-2EB2-4BE4-BDE0-8106C8A05AE8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId40"/>
+  <pageSetup orientation="portrait" r:id="rId51"/>
 </worksheet>
 </file>
 
@@ -22307,7 +22346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2D00-000000000000}">
   <dimension ref="A1:AMK70"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -23310,8 +23349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2E00-000000000000}">
   <dimension ref="A1:AMK71"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23372,7 +23411,7 @@
       <c r="B4" s="7" t="s">
         <v>1689</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="15" t="s">
         <v>103</v>
       </c>
       <c r="D4" s="7" t="s">
@@ -23400,7 +23439,7 @@
       <c r="B6" s="7" t="s">
         <v>1695</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="15" t="s">
         <v>103</v>
       </c>
       <c r="D6" s="7" t="s">
@@ -24774,7 +24813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
   <dimension ref="A1:AMK30"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -25217,7 +25256,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -25873,7 +25912,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>